<commit_message>
bug fix Mac <-> Win compatibility
</commit_message>
<xml_diff>
--- a/examples/custom_lac_promoters.xlsx
+++ b/examples/custom_lac_promoters.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAF64C1-0800-0C4D-9005-D331CAE7F15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OD" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="6">
   <si>
     <t>Time</t>
   </si>
@@ -36,11 +37,14 @@
   <si>
     <t>Blank</t>
   </si>
+  <si>
+    <t>pSEVA634rk∙GFP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,16 +389,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,7 +409,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -414,7 +418,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
@@ -423,7 +427,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>1</v>
@@ -432,7 +436,7 @@
         <v>2</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>1</v>
@@ -441,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>1</v>
@@ -450,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>1</v>
@@ -459,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>4</v>
@@ -471,7 +475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0</v>
       </c>
@@ -536,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -613,7 +617,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.5</v>
       </c>
@@ -690,7 +694,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -767,7 +771,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -844,7 +848,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -921,7 +925,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2.5</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1075,7 +1079,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3.5</v>
       </c>
@@ -1152,7 +1156,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1229,7 +1233,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4.5</v>
       </c>
@@ -1306,7 +1310,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1383,7 +1387,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5.5</v>
       </c>
@@ -1460,7 +1464,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1537,7 +1541,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6.5</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1691,7 +1695,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7.5</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8.5</v>
       </c>
@@ -1922,7 +1926,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1999,7 +2003,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9.5</v>
       </c>
@@ -2076,7 +2080,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -2153,7 +2157,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10.5</v>
       </c>
@@ -2230,7 +2234,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>11</v>
       </c>
@@ -2307,7 +2311,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>11.5</v>
       </c>
@@ -2384,7 +2388,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12</v>
       </c>
@@ -2461,7 +2465,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>12.5</v>
       </c>
@@ -2538,7 +2542,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>13</v>
       </c>
@@ -2615,7 +2619,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13.5</v>
       </c>
@@ -2692,7 +2696,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>14</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>14.5</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>15</v>
       </c>
@@ -2923,7 +2927,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>15.5</v>
       </c>
@@ -3000,7 +3004,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>16</v>
       </c>
@@ -3077,7 +3081,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>16.5</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>17</v>
       </c>
@@ -3231,7 +3235,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>17.5</v>
       </c>
@@ -3308,7 +3312,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>18</v>
       </c>
@@ -3385,7 +3389,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>18.5</v>
       </c>
@@ -3462,7 +3466,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>19</v>
       </c>
@@ -3539,7 +3543,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>19.5</v>
       </c>
@@ -3616,7 +3620,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20</v>
       </c>
@@ -3693,7 +3697,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20.5</v>
       </c>
@@ -3770,7 +3774,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>21</v>
       </c>
@@ -3847,7 +3851,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>21.5</v>
       </c>
@@ -3924,7 +3928,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>22</v>
       </c>
@@ -4001,7 +4005,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22.5</v>
       </c>
@@ -4078,7 +4082,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>23</v>
       </c>
@@ -4155,7 +4159,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>23.5</v>
       </c>
@@ -4232,7 +4236,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>24</v>
       </c>
@@ -4309,7 +4313,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>24.5</v>
       </c>
@@ -4386,7 +4390,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>25</v>
       </c>
@@ -4463,7 +4467,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>25.5</v>
       </c>
@@ -4540,7 +4544,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>26</v>
       </c>
@@ -4617,7 +4621,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>26.5</v>
       </c>
@@ -4694,7 +4698,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>27</v>
       </c>
@@ -4771,7 +4775,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>27.5</v>
       </c>
@@ -4848,7 +4852,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>28</v>
       </c>
@@ -4925,7 +4929,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>28.5</v>
       </c>
@@ -5002,7 +5006,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>29</v>
       </c>
@@ -5079,7 +5083,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>29.5</v>
       </c>
@@ -5156,7 +5160,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>30</v>
       </c>
@@ -5233,7 +5237,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>30.5</v>
       </c>
@@ -5310,7 +5314,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>31</v>
       </c>
@@ -5387,7 +5391,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>31.5</v>
       </c>
@@ -5464,7 +5468,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>32</v>
       </c>
@@ -5541,7 +5545,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>32.5</v>
       </c>
@@ -5618,7 +5622,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>33</v>
       </c>
@@ -5695,7 +5699,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>33.5</v>
       </c>
@@ -5772,7 +5776,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>34</v>
       </c>
@@ -5849,7 +5853,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>34.5</v>
       </c>
@@ -5926,7 +5930,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>35</v>
       </c>
@@ -6003,7 +6007,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>35.5</v>
       </c>
@@ -6080,7 +6084,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>36</v>
       </c>
@@ -6157,7 +6161,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>36.5</v>
       </c>
@@ -6234,7 +6238,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>37</v>
       </c>
@@ -6311,7 +6315,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>37.5</v>
       </c>
@@ -6388,7 +6392,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>38</v>
       </c>
@@ -6465,7 +6469,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>38.5</v>
       </c>
@@ -6542,7 +6546,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>39</v>
       </c>
@@ -6619,7 +6623,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>39.5</v>
       </c>
@@ -6696,7 +6700,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>40</v>
       </c>
@@ -6773,7 +6777,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>40.5</v>
       </c>
@@ -6850,7 +6854,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>41</v>
       </c>
@@ -6927,7 +6931,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>41.5</v>
       </c>
@@ -7004,7 +7008,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>42</v>
       </c>
@@ -7087,16 +7091,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7173,7 +7177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0</v>
       </c>
@@ -7238,7 +7242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -7315,7 +7319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.5</v>
       </c>
@@ -7392,7 +7396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -7469,7 +7473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -7546,7 +7550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -7623,7 +7627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2.5</v>
       </c>
@@ -7700,7 +7704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -7777,7 +7781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3.5</v>
       </c>
@@ -7854,7 +7858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -7931,7 +7935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4.5</v>
       </c>
@@ -8008,7 +8012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -8085,7 +8089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5.5</v>
       </c>
@@ -8162,7 +8166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -8239,7 +8243,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6.5</v>
       </c>
@@ -8316,7 +8320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -8393,7 +8397,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7.5</v>
       </c>
@@ -8470,7 +8474,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
@@ -8547,7 +8551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8.5</v>
       </c>
@@ -8624,7 +8628,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -8701,7 +8705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9.5</v>
       </c>
@@ -8778,7 +8782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -8855,7 +8859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10.5</v>
       </c>
@@ -8932,7 +8936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>11</v>
       </c>
@@ -9009,7 +9013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>11.5</v>
       </c>
@@ -9086,7 +9090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12</v>
       </c>
@@ -9163,7 +9167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>12.5</v>
       </c>
@@ -9240,7 +9244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>13</v>
       </c>
@@ -9317,7 +9321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13.5</v>
       </c>
@@ -9394,7 +9398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>14</v>
       </c>
@@ -9471,7 +9475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>14.5</v>
       </c>
@@ -9548,7 +9552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>15</v>
       </c>
@@ -9625,7 +9629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>15.5</v>
       </c>
@@ -9702,7 +9706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>16</v>
       </c>
@@ -9779,7 +9783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>16.5</v>
       </c>
@@ -9856,7 +9860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>17</v>
       </c>
@@ -9933,7 +9937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>17.5</v>
       </c>
@@ -10010,7 +10014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>18</v>
       </c>
@@ -10087,7 +10091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>18.5</v>
       </c>
@@ -10164,7 +10168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>19</v>
       </c>
@@ -10241,7 +10245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>19.5</v>
       </c>
@@ -10318,7 +10322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20</v>
       </c>
@@ -10395,7 +10399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20.5</v>
       </c>
@@ -10472,7 +10476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>21</v>
       </c>
@@ -10549,7 +10553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>21.5</v>
       </c>
@@ -10626,7 +10630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>22</v>
       </c>
@@ -10703,7 +10707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22.5</v>
       </c>
@@ -10780,7 +10784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>23</v>
       </c>
@@ -10857,7 +10861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>23.5</v>
       </c>
@@ -10934,7 +10938,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>24</v>
       </c>
@@ -11011,7 +11015,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>24.5</v>
       </c>
@@ -11088,7 +11092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>25</v>
       </c>
@@ -11165,7 +11169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>25.5</v>
       </c>
@@ -11242,7 +11246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>26</v>
       </c>
@@ -11319,7 +11323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>26.5</v>
       </c>
@@ -11396,7 +11400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>27</v>
       </c>
@@ -11473,7 +11477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>27.5</v>
       </c>
@@ -11550,7 +11554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>28</v>
       </c>
@@ -11627,7 +11631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>28.5</v>
       </c>
@@ -11704,7 +11708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>29</v>
       </c>
@@ -11781,7 +11785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>29.5</v>
       </c>
@@ -11858,7 +11862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>30</v>
       </c>
@@ -11935,7 +11939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>30.5</v>
       </c>
@@ -12012,7 +12016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>31</v>
       </c>
@@ -12089,7 +12093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>31.5</v>
       </c>
@@ -12166,7 +12170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>32</v>
       </c>
@@ -12243,7 +12247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>32.5</v>
       </c>
@@ -12320,7 +12324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>33</v>
       </c>
@@ -12397,7 +12401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>33.5</v>
       </c>
@@ -12474,7 +12478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>34</v>
       </c>
@@ -12551,7 +12555,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>34.5</v>
       </c>
@@ -12628,7 +12632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>35</v>
       </c>
@@ -12705,7 +12709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>35.5</v>
       </c>
@@ -12782,7 +12786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>36</v>
       </c>
@@ -12859,7 +12863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>36.5</v>
       </c>
@@ -12936,7 +12940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>37</v>
       </c>
@@ -13013,7 +13017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>37.5</v>
       </c>
@@ -13090,7 +13094,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>38</v>
       </c>
@@ -13167,7 +13171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>38.5</v>
       </c>
@@ -13244,7 +13248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>39</v>
       </c>
@@ -13321,7 +13325,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>39.5</v>
       </c>
@@ -13398,7 +13402,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>40</v>
       </c>
@@ -13475,7 +13479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>40.5</v>
       </c>
@@ -13552,7 +13556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>41</v>
       </c>
@@ -13629,7 +13633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>41.5</v>
       </c>
@@ -13706,7 +13710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
renamed column headers in example file for compatibility
</commit_message>
<xml_diff>
--- a/examples/custom_lac_promoters.xlsx
+++ b/examples/custom_lac_promoters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAF64C1-0800-0C4D-9005-D331CAE7F15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457700F4-CA97-D442-AEEE-E32022F29955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="3080" windowWidth="22260" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OD" sheetId="1" r:id="rId1"/>
@@ -21,24 +21,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="5">
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>pSEVA634∙GFP</t>
-  </si>
-  <si>
-    <t>pSEVA634r∙GFP</t>
-  </si>
-  <si>
-    <t>pSEVA634rκ∙GFP</t>
   </si>
   <si>
     <t>Blank</t>
   </si>
   <si>
-    <t>pSEVA634rk∙GFP</t>
+    <t>pSEVA634-GFP</t>
+  </si>
+  <si>
+    <t>pSEVA634r-GFP</t>
+  </si>
+  <si>
+    <t>pSEVA634rk-GFP</t>
   </si>
 </sst>
 </file>
@@ -392,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -403,76 +400,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
@@ -7094,8 +7091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7105,76 +7102,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>